<commit_message>
fixed footer wrong placement on landing page
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_11_Mar.xlsx
+++ b/other/Project_TimeLine_2021_11_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE4590-ADB0-475A-B28F-517702F00E28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E234096B-DFA8-411E-82FC-5BCBA4FFF290}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>S/N</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Creating functionality for groups</t>
+  </si>
+  <si>
+    <t>Front-end: Data charts</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,42 +919,37 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="I17" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="H18" t="s">
-        <v>19</v>
+      <c r="I18" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -959,17 +957,36 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="H20" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>